<commit_message>
data till 19 Feb 8AM
</commit_message>
<xml_diff>
--- a/Febuary2021.xlsx
+++ b/Febuary2021.xlsx
@@ -48,6 +48,29 @@
       </text>
     </comment>
     <comment ref="V16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+1040-Auto
+1040-Auto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z53" authorId="0">
       <text>
         <r>
           <rPr>
@@ -753,9 +776,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -782,9 +805,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -799,7 +821,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -807,7 +859,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,6 +903,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -853,29 +920,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -892,28 +937,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1017,7 +1040,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,19 +1082,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1053,7 +1106,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1071,7 +1124,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,7 +1142,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1095,13 +1154,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1113,43 +1166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1161,31 +1178,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,6 +1209,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1222,6 +1245,15 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1265,6 +1297,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1282,9 +1323,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1303,32 +1346,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1346,130 +1369,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1925,11 +1948,11 @@
   <dimension ref="A1:AS114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="X57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="Y17" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E63" sqref="E63"/>
+      <selection pane="bottomRight" activeCell="AA37" sqref="AA37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2067,22 +2090,22 @@
       <c r="A2" s="13"/>
       <c r="B2" s="25">
         <f>SUM(F3:F121)</f>
-        <v>951700</v>
+        <v>991700</v>
       </c>
       <c r="D2" s="14">
         <f>SUM(G3:G121)</f>
-        <v>814840</v>
+        <v>856440</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="25">
         <f t="shared" ref="F2:F18" si="0">G2/1.04+H2</f>
-        <v>951700</v>
+        <v>991700</v>
       </c>
       <c r="G2" s="14">
         <f t="shared" ref="G2:G28" si="1">SUM(I2:AM2)</f>
-        <v>814840</v>
+        <v>856440</v>
       </c>
       <c r="H2" s="26">
         <f t="shared" ref="H2:AJ2" si="2">SUM(H3:H121)</f>
@@ -2158,11 +2181,11 @@
       </c>
       <c r="Z2" s="10">
         <f t="shared" si="2"/>
-        <v>11440</v>
+        <v>24960</v>
       </c>
       <c r="AA2" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28080</v>
       </c>
       <c r="AB2" s="10">
         <f t="shared" si="2"/>
@@ -2346,7 +2369,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="7" s="11" customFormat="1" spans="1:25">
+    <row r="7" s="11" customFormat="1" spans="1:27">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -2361,11 +2384,11 @@
       </c>
       <c r="F7" s="10">
         <f t="shared" si="0"/>
-        <v>47000</v>
+        <v>51000</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="1"/>
-        <v>37440</v>
+        <v>41600</v>
       </c>
       <c r="H7" s="27">
         <v>11000</v>
@@ -2418,8 +2441,14 @@
       <c r="Y7" s="11">
         <v>2080</v>
       </c>
-    </row>
-    <row r="8" s="11" customFormat="1" spans="1:20">
+      <c r="Z7" s="11">
+        <v>2080</v>
+      </c>
+      <c r="AA7" s="11">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="8" s="11" customFormat="1" spans="1:27">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -2434,11 +2463,11 @@
       </c>
       <c r="F8" s="10">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="1"/>
-        <v>4160</v>
+        <v>6240</v>
       </c>
       <c r="H8" s="27">
         <v>0</v>
@@ -2447,6 +2476,9 @@
         <v>2080</v>
       </c>
       <c r="T8" s="11">
+        <v>2080</v>
+      </c>
+      <c r="AA8" s="11">
         <v>2080</v>
       </c>
     </row>
@@ -2800,7 +2832,7 @@
       <c r="Z18" s="33"/>
       <c r="AA18" s="33"/>
     </row>
-    <row r="19" s="11" customFormat="1" spans="1:22">
+    <row r="19" s="11" customFormat="1" spans="1:27">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -2812,11 +2844,11 @@
       </c>
       <c r="F19" s="10">
         <f t="shared" ref="F19:F82" si="3">G19/1.04+H19</f>
-        <v>8000</v>
+        <v>11000</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" si="1"/>
-        <v>9360</v>
+        <v>12480</v>
       </c>
       <c r="H19" s="27">
         <v>-1000</v>
@@ -2828,6 +2860,9 @@
         <v>3120</v>
       </c>
       <c r="V19" s="11">
+        <v>3120</v>
+      </c>
+      <c r="AA19" s="11">
         <v>3120</v>
       </c>
     </row>
@@ -2961,7 +2996,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="24" s="11" customFormat="1" spans="1:23">
+    <row r="24" s="11" customFormat="1" spans="1:27">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -2973,11 +3008,11 @@
       </c>
       <c r="F24" s="10">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="G24" s="10">
         <f t="shared" si="1"/>
-        <v>5200</v>
+        <v>6240</v>
       </c>
       <c r="H24" s="27">
         <v>1000</v>
@@ -2995,6 +3030,9 @@
         <v>1040</v>
       </c>
       <c r="W24" s="11">
+        <v>1040</v>
+      </c>
+      <c r="AA24" s="11">
         <v>1040</v>
       </c>
     </row>
@@ -3035,7 +3073,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="26" s="11" customFormat="1" spans="1:24">
+    <row r="26" s="11" customFormat="1" spans="1:27">
       <c r="A26" s="11">
         <v>24</v>
       </c>
@@ -3047,11 +3085,11 @@
       </c>
       <c r="F26" s="10">
         <f t="shared" si="3"/>
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="G26" s="10">
         <f t="shared" si="1"/>
-        <v>26000</v>
+        <v>31200</v>
       </c>
       <c r="H26" s="27">
         <v>0</v>
@@ -3069,6 +3107,9 @@
         <v>5200</v>
       </c>
       <c r="X26" s="11">
+        <v>5200</v>
+      </c>
+      <c r="AA26" s="11">
         <v>5200</v>
       </c>
     </row>
@@ -3409,7 +3450,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="37" s="11" customFormat="1" spans="1:26">
+    <row r="37" s="11" customFormat="1" spans="1:27">
       <c r="A37" s="11">
         <v>35</v>
       </c>
@@ -3421,11 +3462,11 @@
       </c>
       <c r="F37" s="10">
         <f t="shared" si="3"/>
-        <v>21000</v>
+        <v>24000</v>
       </c>
       <c r="G37" s="10">
         <f t="shared" si="4"/>
-        <v>21840</v>
+        <v>24960</v>
       </c>
       <c r="H37" s="27">
         <v>0</v>
@@ -3449,6 +3490,9 @@
         <v>3120</v>
       </c>
       <c r="Z37" s="11">
+        <v>3120</v>
+      </c>
+      <c r="AA37" s="11">
         <v>3120</v>
       </c>
     </row>
@@ -3536,7 +3580,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="41" s="11" customFormat="1" spans="1:23">
+    <row r="41" s="11" customFormat="1" spans="1:27">
       <c r="A41" s="11">
         <v>39</v>
       </c>
@@ -3548,11 +3592,11 @@
       </c>
       <c r="F41" s="10">
         <f t="shared" si="3"/>
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="G41" s="10">
         <f t="shared" si="4"/>
-        <v>6240</v>
+        <v>8320</v>
       </c>
       <c r="H41" s="27">
         <v>2000</v>
@@ -3564,6 +3608,9 @@
         <v>2080</v>
       </c>
       <c r="W41" s="11">
+        <v>2080</v>
+      </c>
+      <c r="AA41" s="11">
         <v>2080</v>
       </c>
     </row>
@@ -3669,7 +3716,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="45" s="11" customFormat="1" spans="1:24">
+    <row r="45" s="11" customFormat="1" spans="1:26">
       <c r="A45" s="11">
         <v>43</v>
       </c>
@@ -3681,11 +3728,11 @@
       </c>
       <c r="F45" s="10">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>18000</v>
       </c>
       <c r="G45" s="10">
         <f t="shared" si="5"/>
-        <v>15600</v>
+        <v>18720</v>
       </c>
       <c r="H45" s="27">
         <v>0</v>
@@ -3703,6 +3750,9 @@
         <v>3120</v>
       </c>
       <c r="X45" s="11">
+        <v>3120</v>
+      </c>
+      <c r="Z45" s="11">
         <v>3120</v>
       </c>
     </row>
@@ -3947,11 +3997,11 @@
       </c>
       <c r="F53" s="10">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>13000</v>
       </c>
       <c r="G53" s="10">
         <f t="shared" si="5"/>
-        <v>12480</v>
+        <v>13520</v>
       </c>
       <c r="H53" s="27">
         <v>0</v>
@@ -3990,10 +4040,10 @@
         <v>1040</v>
       </c>
       <c r="Z53" s="11">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="54" s="11" customFormat="1" spans="1:24">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="54" s="11" customFormat="1" spans="1:26">
       <c r="A54" s="11">
         <v>52</v>
       </c>
@@ -4005,11 +4055,11 @@
       </c>
       <c r="F54" s="10">
         <f t="shared" si="3"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="G54" s="10">
         <f t="shared" si="5"/>
-        <v>8320</v>
+        <v>10400</v>
       </c>
       <c r="H54" s="27">
         <v>2000</v>
@@ -4024,6 +4074,9 @@
         <v>2080</v>
       </c>
       <c r="X54" s="11">
+        <v>2080</v>
+      </c>
+      <c r="Z54" s="11">
         <v>2080</v>
       </c>
     </row>
@@ -4204,7 +4257,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="61" s="11" customFormat="1" spans="1:24">
+    <row r="61" s="11" customFormat="1" spans="1:27">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -4216,11 +4269,11 @@
       </c>
       <c r="F61" s="10">
         <f t="shared" si="3"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="G61" s="10">
         <f t="shared" si="5"/>
-        <v>10400</v>
+        <v>12480</v>
       </c>
       <c r="H61" s="27">
         <v>0</v>
@@ -4238,6 +4291,9 @@
         <v>2080</v>
       </c>
       <c r="X61" s="11">
+        <v>2080</v>
+      </c>
+      <c r="AA61" s="11">
         <v>2080</v>
       </c>
     </row>
@@ -4327,7 +4383,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="65" s="11" customFormat="1" spans="1:15">
+    <row r="65" s="11" customFormat="1" spans="1:26">
       <c r="A65" s="11">
         <v>63</v>
       </c>
@@ -4342,11 +4398,11 @@
       </c>
       <c r="F65" s="10">
         <f t="shared" si="3"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="G65" s="10">
         <f t="shared" si="5"/>
-        <v>2080</v>
+        <v>4160</v>
       </c>
       <c r="H65" s="22">
         <v>2000</v>
@@ -4354,8 +4410,11 @@
       <c r="O65" s="11">
         <v>2080</v>
       </c>
-    </row>
-    <row r="66" s="11" customFormat="1" spans="1:21">
+      <c r="Z65" s="11">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="66" s="11" customFormat="1" spans="1:27">
       <c r="A66" s="11">
         <v>64</v>
       </c>
@@ -4368,11 +4427,11 @@
       </c>
       <c r="F66" s="10">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="G66" s="10">
         <f t="shared" si="5"/>
-        <v>10400</v>
+        <v>12480</v>
       </c>
       <c r="H66" s="27">
         <v>2000</v>
@@ -4390,6 +4449,9 @@
         <v>2080</v>
       </c>
       <c r="U66" s="11">
+        <v>2080</v>
+      </c>
+      <c r="AA66" s="11">
         <v>2080</v>
       </c>
     </row>
@@ -4540,7 +4602,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="72" s="11" customFormat="1" spans="1:23">
+    <row r="72" s="11" customFormat="1" spans="1:27">
       <c r="A72" s="11">
         <v>70</v>
       </c>
@@ -4552,11 +4614,11 @@
       </c>
       <c r="F72" s="10">
         <f t="shared" si="3"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="G72" s="10">
         <f t="shared" si="5"/>
-        <v>26000</v>
+        <v>31200</v>
       </c>
       <c r="H72" s="27">
         <v>5000</v>
@@ -4576,8 +4638,11 @@
       <c r="W72" s="11">
         <v>5200</v>
       </c>
-    </row>
-    <row r="73" s="11" customFormat="1" spans="1:23">
+      <c r="AA72" s="11">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="73" s="11" customFormat="1" spans="1:26">
       <c r="A73" s="11">
         <v>71</v>
       </c>
@@ -4589,11 +4654,11 @@
       </c>
       <c r="F73" s="10">
         <f t="shared" si="3"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="G73" s="10">
         <f t="shared" si="5"/>
-        <v>12480</v>
+        <v>15600</v>
       </c>
       <c r="H73" s="27">
         <v>0</v>
@@ -4608,6 +4673,9 @@
         <v>3120</v>
       </c>
       <c r="W73" s="11">
+        <v>3120</v>
+      </c>
+      <c r="Z73" s="11">
         <v>3120</v>
       </c>
     </row>
@@ -5377,11 +5445,11 @@
   <dimension ref="A1:AM96"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="Q81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="S78" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y101" sqref="Y101"/>
+      <selection pane="bottomRight" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -5522,14 +5590,14 @@
       <c r="E2" s="13"/>
       <c r="F2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>767200</v>
+        <v>803700</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="14">
         <f t="shared" ref="H2:H18" si="0">SUM(I2:AM2)</f>
-        <v>767200</v>
+        <v>803700</v>
       </c>
       <c r="I2" s="10">
         <f t="shared" ref="I2:AJ2" si="1">SUM(I3:I121)</f>
@@ -5601,7 +5669,7 @@
       </c>
       <c r="Z2" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>36500</v>
       </c>
       <c r="AA2" s="10">
         <f t="shared" si="1"/>
@@ -5842,7 +5910,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="8" s="11" customFormat="1" spans="1:11">
+    <row r="8" s="11" customFormat="1" spans="1:26">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -5860,13 +5928,16 @@
       </c>
       <c r="H8" s="10">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="K8" s="11">
         <v>2000</v>
       </c>
-    </row>
-    <row r="9" s="11" customFormat="1" spans="1:18">
+      <c r="Z8" s="11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" s="11" customFormat="1" spans="1:26">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -5884,12 +5955,15 @@
       </c>
       <c r="H9" s="10">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I9" s="11">
         <v>2000</v>
       </c>
       <c r="R9" s="11">
+        <v>2000</v>
+      </c>
+      <c r="Z9" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -5995,7 +6069,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" s="11" customFormat="1" spans="1:21">
+    <row r="13" s="11" customFormat="1" spans="1:26">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -6013,7 +6087,7 @@
       </c>
       <c r="H13" s="10">
         <f t="shared" si="0"/>
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="L13" s="11">
         <v>5000</v>
@@ -6024,8 +6098,11 @@
       <c r="U13" s="11">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" s="11" customFormat="1" spans="1:25">
+      <c r="Z13" s="19">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" s="11" customFormat="1" spans="1:26">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -6049,7 +6126,7 @@
       </c>
       <c r="H14" s="10">
         <f t="shared" si="0"/>
-        <v>33500</v>
+        <v>36500</v>
       </c>
       <c r="I14" s="11">
         <v>4500</v>
@@ -6083,6 +6160,9 @@
       </c>
       <c r="Y14" s="11">
         <v>4000</v>
+      </c>
+      <c r="Z14" s="11">
+        <v>3000</v>
       </c>
     </row>
     <row r="15" s="11" customFormat="1" spans="1:25">
@@ -6175,7 +6255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" s="11" customFormat="1" spans="1:20">
+    <row r="18" s="11" customFormat="1" spans="1:26">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -6190,9 +6270,12 @@
       </c>
       <c r="H18" s="10">
         <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="T18" s="11">
         <v>1000</v>
       </c>
-      <c r="T18" s="11">
+      <c r="Z18" s="11">
         <v>1000</v>
       </c>
     </row>
@@ -6379,7 +6462,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="24" s="11" customFormat="1" spans="1:25">
+    <row r="24" s="11" customFormat="1" spans="1:26">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -6397,7 +6480,7 @@
       </c>
       <c r="H24" s="10">
         <f t="shared" si="2"/>
-        <v>5500</v>
+        <v>6000</v>
       </c>
       <c r="I24" s="11">
         <v>1000</v>
@@ -6415,6 +6498,9 @@
         <v>1000</v>
       </c>
       <c r="Y24" s="11">
+        <v>500</v>
+      </c>
+      <c r="Z24" s="11">
         <v>500</v>
       </c>
     </row>
@@ -6703,7 +6789,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="33" s="11" customFormat="1" spans="1:25">
+    <row r="33" s="11" customFormat="1" spans="1:26">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -6718,7 +6804,7 @@
       </c>
       <c r="H33" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>10000</v>
       </c>
       <c r="I33" s="11">
         <v>1000</v>
@@ -6745,6 +6831,9 @@
         <v>1000</v>
       </c>
       <c r="Y33" s="11">
+        <v>1000</v>
+      </c>
+      <c r="Z33" s="11">
         <v>1000</v>
       </c>
     </row>
@@ -6847,7 +6936,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="37" s="11" customFormat="1" spans="1:25">
+    <row r="37" s="11" customFormat="1" spans="1:26">
       <c r="A37" s="11">
         <v>35</v>
       </c>
@@ -6862,7 +6951,7 @@
       </c>
       <c r="H37" s="10">
         <f t="shared" si="2"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="J37" s="18">
         <v>3000</v>
@@ -6880,6 +6969,9 @@
         <v>3000</v>
       </c>
       <c r="Y37" s="19">
+        <v>3000</v>
+      </c>
+      <c r="Z37" s="19">
         <v>3000</v>
       </c>
     </row>
@@ -6970,7 +7062,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" s="11" customFormat="1" spans="1:16">
+    <row r="41" s="11" customFormat="1" spans="1:26">
       <c r="A41" s="11">
         <v>39</v>
       </c>
@@ -6985,9 +7077,12 @@
       </c>
       <c r="H41" s="10">
         <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+      <c r="P41" s="11">
         <v>4000</v>
       </c>
-      <c r="P41" s="11">
+      <c r="Z41" s="11">
         <v>4000</v>
       </c>
     </row>
@@ -7114,7 +7209,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="46" s="11" customFormat="1" spans="1:18">
+    <row r="46" s="11" customFormat="1" spans="1:26">
       <c r="A46" s="11">
         <v>44</v>
       </c>
@@ -7135,7 +7230,7 @@
       </c>
       <c r="H46" s="10">
         <f t="shared" si="2"/>
-        <v>12000</v>
+        <v>15000</v>
       </c>
       <c r="J46" s="11">
         <v>3000</v>
@@ -7145,6 +7240,9 @@
       </c>
       <c r="R46" s="11">
         <v>6000</v>
+      </c>
+      <c r="Z46" s="19">
+        <v>3000</v>
       </c>
     </row>
     <row r="47" s="11" customFormat="1" spans="1:25">
@@ -7390,7 +7488,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="54" s="11" customFormat="1" spans="1:25">
+    <row r="54" s="11" customFormat="1" spans="1:26">
       <c r="A54" s="11">
         <v>52</v>
       </c>
@@ -7405,7 +7503,7 @@
       </c>
       <c r="H54" s="10">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="I54" s="18">
         <v>2000</v>
@@ -7418,6 +7516,9 @@
       </c>
       <c r="Y54" s="19">
         <v>5000</v>
+      </c>
+      <c r="Z54" s="19">
+        <v>2000</v>
       </c>
     </row>
     <row r="55" s="11" customFormat="1" spans="1:21">
@@ -7909,7 +8010,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="73" s="11" customFormat="1" spans="1:25">
+    <row r="73" s="11" customFormat="1" spans="1:26">
       <c r="A73" s="11">
         <v>71</v>
       </c>
@@ -7924,7 +8025,7 @@
       </c>
       <c r="H73" s="10">
         <f t="shared" si="2"/>
-        <v>9000</v>
+        <v>12000</v>
       </c>
       <c r="K73" s="11">
         <v>3000</v>
@@ -7933,6 +8034,9 @@
         <v>3000</v>
       </c>
       <c r="Y73" s="19">
+        <v>3000</v>
+      </c>
+      <c r="Z73" s="11">
         <v>3000</v>
       </c>
     </row>
@@ -8014,7 +8118,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="77" s="11" customFormat="1" spans="1:25">
+    <row r="77" s="11" customFormat="1" spans="1:26">
       <c r="A77" s="11">
         <v>75</v>
       </c>
@@ -8038,7 +8142,7 @@
       </c>
       <c r="H77" s="10">
         <f t="shared" si="2"/>
-        <v>8600</v>
+        <v>10100</v>
       </c>
       <c r="J77" s="11">
         <v>1200</v>
@@ -8060,6 +8164,9 @@
       </c>
       <c r="Y77" s="11">
         <v>1600</v>
+      </c>
+      <c r="Z77" s="11">
+        <v>1500</v>
       </c>
     </row>
     <row r="78" s="11" customFormat="1" spans="1:21">
@@ -8098,7 +8205,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="79" s="11" customFormat="1" spans="1:23">
+    <row r="79" s="11" customFormat="1" spans="1:26">
       <c r="A79" s="11">
         <v>77</v>
       </c>
@@ -8119,7 +8226,7 @@
       </c>
       <c r="H79" s="10">
         <f t="shared" si="2"/>
-        <v>11000</v>
+        <v>14500</v>
       </c>
       <c r="I79" s="11">
         <v>2000</v>
@@ -8135,6 +8242,9 @@
       </c>
       <c r="W79" s="11">
         <v>2000</v>
+      </c>
+      <c r="Z79" s="11">
+        <v>3500</v>
       </c>
     </row>
     <row r="80" s="11" customFormat="1" spans="1:8">
@@ -8314,7 +8424,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="88" s="11" customFormat="1" spans="1:19">
+    <row r="88" s="11" customFormat="1" spans="1:26">
       <c r="A88" s="11">
         <v>86</v>
       </c>
@@ -8329,9 +8439,12 @@
       </c>
       <c r="H88" s="10">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="S88" s="18">
+        <v>2000</v>
+      </c>
+      <c r="Z88" s="11">
         <v>2000</v>
       </c>
     </row>
@@ -8486,7 +8599,7 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -8522,7 +8635,7 @@
       </c>
       <c r="D2" s="6">
         <f>Orders!F2-Collection!H2</f>
-        <v>184500</v>
+        <v>188000</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8597,7 +8710,7 @@
       </c>
       <c r="D7" s="9">
         <f>Orders!F7-Collection!H7</f>
-        <v>12000</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8627,7 +8740,7 @@
       </c>
       <c r="D9" s="9">
         <f>Orders!F9-Collection!H9</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -8687,7 +8800,7 @@
       </c>
       <c r="D13" s="9">
         <f>Orders!F13-Collection!H13</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -8702,7 +8815,7 @@
       </c>
       <c r="D14" s="9">
         <f>Orders!F14-Collection!H14</f>
-        <v>7000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -8756,7 +8869,7 @@
       </c>
       <c r="D18" s="9">
         <f>Orders!F18-Collection!H18</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -8771,7 +8884,7 @@
       </c>
       <c r="D19" s="9">
         <f>Orders!F19-Collection!H19</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -8846,7 +8959,7 @@
       </c>
       <c r="D24" s="9">
         <f>Orders!F24-Collection!H24</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -8876,7 +8989,7 @@
       </c>
       <c r="D26" s="9">
         <f>Orders!F26-Collection!H26</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8975,7 +9088,7 @@
       </c>
       <c r="D33" s="9">
         <f>Orders!F33-Collection!H33</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -9083,7 +9196,7 @@
       </c>
       <c r="D41" s="9">
         <f>Orders!F41-Collection!H41</f>
-        <v>4000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -9137,7 +9250,7 @@
       </c>
       <c r="D45" s="9">
         <f>Orders!F45-Collection!H45</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -9150,7 +9263,7 @@
       </c>
       <c r="D46" s="9">
         <f>Orders!F46-Collection!H46</f>
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -9245,7 +9358,7 @@
       </c>
       <c r="D53" s="9">
         <f>Orders!F53-Collection!H53</f>
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -9353,7 +9466,7 @@
       </c>
       <c r="D61" s="9">
         <f>Orders!F61-Collection!H61</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -9413,7 +9526,7 @@
       </c>
       <c r="D65" s="9">
         <f>Orders!F65-Collection!H65</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -9426,7 +9539,7 @@
       </c>
       <c r="D66" s="9">
         <f>Orders!F66-Collection!H66</f>
-        <v>4000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -9504,7 +9617,7 @@
       </c>
       <c r="D72" s="9">
         <f>Orders!F72-Collection!H72</f>
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -9575,7 +9688,7 @@
       </c>
       <c r="D77" s="9">
         <f>Orders!F77-Collection!H77</f>
-        <v>2400</v>
+        <v>900</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -9601,7 +9714,7 @@
       </c>
       <c r="D79" s="9">
         <f>Orders!F79-Collection!H79</f>
-        <v>4000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -9718,7 +9831,7 @@
       </c>
       <c r="D88" s="9">
         <f>Orders!F88-Collection!H88</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -9812,9 +9925,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D96">
-    <extLst/>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>